<commit_message>
Update-MC Inv Home V
</commit_message>
<xml_diff>
--- a/bin/Debug/Template/InventoryLabel_SD_Template.xlsx
+++ b/bin/Debug/Template/InventoryLabel_SD_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Current Works\MC-Dept-App\bin\Debug\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Project\My C# project\MC-Dept-App\bin\Debug\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98926BB-2846-4C3D-A3AD-A6B147C7B51B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49E2A54-BFBE-4285-8602-F5C126D8B8A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{CC1B00A2-45D8-49ED-889F-8263ED2BB9E1}"/>
+    <workbookView xWindow="2430" yWindow="1980" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{CC1B00A2-45D8-49ED-889F-8263ED2BB9E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Wire" sheetId="5" r:id="rId1"/>
@@ -32,27 +32,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
-  <si>
-    <t>BobbinCode</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
   <si>
     <t>Remain KG</t>
-  </si>
-  <si>
-    <t>RemainQty</t>
   </si>
   <si>
     <t>No.</t>
   </si>
   <si>
-    <t>fadfdafaffafda</t>
+    <t>Bobbin Code</t>
   </si>
   <si>
-    <t>23,500 m (5 Bobbins)</t>
-  </si>
-  <si>
-    <t>23,500 Pcs (5 Bobbins/Reels)</t>
+    <t>Remain Qty</t>
   </si>
 </sst>
 </file>
@@ -60,9 +51,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="167" formatCode="#,##0\ &quot;m&quot;"/>
-    <numFmt numFmtId="170" formatCode="#,##0.00\ &quot;Kg&quot;"/>
-    <numFmt numFmtId="171" formatCode="#,##0\ &quot;Pcs&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0\ &quot;m&quot;"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;Kg&quot;"/>
+    <numFmt numFmtId="166" formatCode="#,##0\ &quot;Pcs&quot;"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -182,33 +173,30 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -216,8 +204,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -297,7 +288,8 @@
               <a:ea typeface="Calibri"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
-            <a:t>24-03-2025</a:t>
+            <a:pPr algn="l"/>
+            <a:t> </a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1100" b="1">
             <a:solidFill>
@@ -840,7 +832,8 @@
               <a:ea typeface="Calibri"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
-            <a:t>3000</a:t>
+            <a:pPr algn="l"/>
+            <a:t> </a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1100" b="0"/>
         </a:p>
@@ -907,7 +900,8 @@
               <a:ea typeface="Calibri"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
-            <a:t>fadfdafaffafda</a:t>
+            <a:pPr algn="l"/>
+            <a:t> </a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1100" b="0"/>
         </a:p>
@@ -974,7 +968,8 @@
               <a:ea typeface="Calibri"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
-            <a:t>23,500 m (5 Bobbins)</a:t>
+            <a:pPr algn="l"/>
+            <a:t> </a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1100" b="0"/>
         </a:p>
@@ -982,6 +977,380 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>29766</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>11906</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1004216</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="9" name="Group 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABCECA08-A845-4A3A-AE71-D576D11428F6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="29766" y="2333625"/>
+          <a:ext cx="3242591" cy="726281"/>
+          <a:chOff x="95250" y="2684860"/>
+          <a:chExt cx="3482578" cy="779859"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="10" name="Rectangle 9">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11827E46-FA0D-AA72-0A58-E8C73A0A5C93}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="95250" y="2684860"/>
+            <a:ext cx="1160859" cy="214313"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1000" b="1">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Approved</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="16" name="Rectangle 15">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F3AAD06-A784-CA13-04FF-EF8BB938289D}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1256109" y="2684860"/>
+            <a:ext cx="1160859" cy="214313"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1000" b="1">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Confirmed</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="17" name="Rectangle 16">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0FE6127-83BC-ED61-8C99-AA7D385DA4DD}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2416969" y="2684860"/>
+            <a:ext cx="1160859" cy="214313"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1000" b="1">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Checked</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="18" name="Rectangle 17">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B037484-1C59-841E-A0F8-B656D296BA04}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="95250" y="2899172"/>
+            <a:ext cx="1160859" cy="565547"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="19" name="Rectangle 18">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7ABB5055-0DA7-AFFF-624B-AEF9EAB4237F}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1256109" y="2899172"/>
+            <a:ext cx="1160859" cy="565547"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="20" name="Rectangle 19">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FD22C47-1D0F-6BFC-87BA-9EA1E8EFDBF3}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2416969" y="2899172"/>
+            <a:ext cx="1160859" cy="565547"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1046,7 +1415,8 @@
               <a:ea typeface="Calibri"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
-            <a:t>24-03-2025</a:t>
+            <a:pPr algn="l"/>
+            <a:t> </a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1100" b="1">
             <a:solidFill>
@@ -1589,7 +1959,8 @@
               <a:ea typeface="Calibri"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
-            <a:t>3000</a:t>
+            <a:pPr algn="l"/>
+            <a:t> </a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1100" b="0"/>
         </a:p>
@@ -1656,7 +2027,8 @@
               <a:ea typeface="Calibri"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
-            <a:t>fadfdafaffafda</a:t>
+            <a:pPr algn="l"/>
+            <a:t> </a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1100" b="0"/>
         </a:p>
@@ -1723,7 +2095,8 @@
               <a:ea typeface="Calibri"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
-            <a:t>23,500 Pcs (5 Bobbins/Reels)</a:t>
+            <a:pPr algn="l"/>
+            <a:t> </a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1100" b="0"/>
         </a:p>
@@ -1731,6 +2104,380 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>29765</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>11906</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1004941</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="20" name="Group 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{743253D4-53D7-D614-43E7-82CEA214C83B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="29765" y="2335077"/>
+          <a:ext cx="3242591" cy="726281"/>
+          <a:chOff x="95250" y="2684860"/>
+          <a:chExt cx="3482578" cy="779859"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="14" name="Rectangle 13">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4697678E-CCF9-C8C8-AE29-421049FA5850}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="95250" y="2684860"/>
+            <a:ext cx="1160859" cy="214313"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1000" b="1">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Approved</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="15" name="Rectangle 14">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E9BF63E-5F31-B462-5514-BD0CD002B953}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1256109" y="2684860"/>
+            <a:ext cx="1160859" cy="214313"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1000" b="1">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Confirmed</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="16" name="Rectangle 15">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FB05F82-2346-7D3E-387D-81C0D9EE26EE}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2416969" y="2684860"/>
+            <a:ext cx="1160859" cy="214313"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1000" b="1">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Checked</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="17" name="Rectangle 16">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8698D8D9-72BF-653D-B9A2-3D6B7D3F0B09}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="95250" y="2899172"/>
+            <a:ext cx="1160859" cy="565547"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="18" name="Rectangle 17">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BDB06F4-4618-03F5-788A-181A803C4A38}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1256109" y="2899172"/>
+            <a:ext cx="1160859" cy="565547"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="19" name="Rectangle 18">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44C43DCF-B058-EFC8-6D27-5CFD46D4C27B}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2416969" y="2899172"/>
+            <a:ext cx="1160859" cy="565547"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2034,7 +2781,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:D9"/>
+      <selection activeCell="C2" sqref="C2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2046,76 +2793,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
-        <f ca="1">NOW()</f>
-        <v>45740.771097685189</v>
-      </c>
+      <c r="A1" s="1"/>
       <c r="B1" s="2" t="str">
-        <f ca="1">IF(A1&lt;&gt;"",TEXT(A1,"dd-mm-yyyy"),"")</f>
-        <v>24-03-2025</v>
+        <f>IF(A1&lt;&gt;"",TEXT(A1,"dd-mm-yyyy"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="1:4" ht="42.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+    </row>
+    <row r="5" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="6">
-        <f>IF(A2&lt;&gt;"",A2,"")</f>
-        <v>1</v>
+      <c r="B8" s="5" t="s">
+        <v>2</v>
       </c>
-      <c r="D2" s="6"/>
-    </row>
-    <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="1:4" ht="42.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A4" s="4" t="str">
-        <f>IF(A2&lt;&gt;"","*"&amp;A2&amp;"*","")</f>
-        <v>*1*</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="5">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="8" t="s">
+      <c r="C8" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>2</v>
+      <c r="D8" s="5" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="9"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="6"/>
     </row>
   </sheetData>
   <autoFilter ref="A8:D8" xr:uid="{5A7028D1-B92E-416F-A083-78DEEB2FAA38}"/>
@@ -2140,8 +2870,8 @@
   </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2153,74 +2883,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
-        <f ca="1">NOW()</f>
-        <v>45740.771097685189</v>
-      </c>
+      <c r="A1" s="1"/>
       <c r="B1" s="2" t="str">
-        <f ca="1">IF(A1&lt;&gt;"",TEXT(A1,"dd-mm-yyyy"),"")</f>
-        <v>24-03-2025</v>
+        <f>IF(A1&lt;&gt;"",TEXT(A1,"dd-mm-yyyy"),"")</f>
+        <v/>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="1:4" ht="42.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+    </row>
+    <row r="5" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="6">
-        <f>IF(A2&lt;&gt;"",A2,"")</f>
-        <v>1</v>
+      <c r="B8" s="14" t="s">
+        <v>2</v>
       </c>
-      <c r="D2" s="6"/>
-    </row>
-    <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="1:4" ht="42.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A4" s="4" t="str">
-        <f>IF(A2&lt;&gt;"","*"&amp;A2&amp;"*","")</f>
-        <v>*1*</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="5">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="C8" s="15"/>
+      <c r="D8" s="5" t="s">
         <v>3</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="8" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="15"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="8"/>
     </row>
   </sheetData>
   <autoFilter ref="A8:D8" xr:uid="{E8573112-A100-4DFB-A880-CF5E1A80A35F}">

</xml_diff>

<commit_message>
Update-MC Inv Home VI
</commit_message>
<xml_diff>
--- a/bin/Debug/Template/InventoryLabel_SD_Template.xlsx
+++ b/bin/Debug/Template/InventoryLabel_SD_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Project\My C# project\MC-Dept-App\bin\Debug\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Current Works\MC-Dept-App\bin\Debug\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49E2A54-BFBE-4285-8602-F5C126D8B8A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B29629E-435B-47B7-90B7-4D1574E206B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2430" yWindow="1980" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{CC1B00A2-45D8-49ED-889F-8263ED2BB9E1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{CC1B00A2-45D8-49ED-889F-8263ED2BB9E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Wire" sheetId="5" r:id="rId1"/>
@@ -2871,7 +2871,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D3"/>
+      <selection activeCell="A4" sqref="A4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>